<commit_message>
linked my stylesheets, wrote my h1
</commit_message>
<xml_diff>
--- a/planetData.xlsx
+++ b/planetData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2242a4c7a55b2ae1/Homework/ITM 361 - Web Development/Github/ITMD361_Lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{28DD3D4B-184B-43DC-A3CF-A4BFF32B08D4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{32DDA8C2-1474-4867-B5E3-D5AD3FDC3CA8}"/>
   </bookViews>
@@ -147,7 +148,9 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +468,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fine-tuned the padding on my table headers to account for the 960 grid layout.
the 960 grid system provides either a 12 or 16 column layout option. Unfortunately, I have 5 columns, which does not divide evenly into 12 or 16. Therefore, I had to calculate the leftover space and increase my margin accordingly to get the table headers aligned exactly the way I wanted them.
</commit_message>
<xml_diff>
--- a/planetData.xlsx
+++ b/planetData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2242a4c7a55b2ae1/Homework/ITM 361 - Web Development/Github/ITMD361_Lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{28DD3D4B-184B-43DC-A3CF-A4BFF32B08D4}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{5A13FC9C-BB62-499F-8090-1424E5FBE2E4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{32DDA8C2-1474-4867-B5E3-D5AD3FDC3CA8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Earth </t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t>1.02 x 1026</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Padding</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>Remainder</t>
+  </si>
+  <si>
+    <t>Per</t>
   </si>
 </sst>
 </file>
@@ -465,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549B531D-7886-49E9-AE68-35EA5B5D227D}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +497,7 @@
     <col min="4" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -496,7 +514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -513,7 +531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -530,7 +548,7 @@
         <v>49528</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -547,7 +565,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -564,7 +582,7 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -581,7 +599,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -598,7 +616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -613,6 +631,50 @@
       </c>
       <c r="E8" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>960</v>
+      </c>
+      <c r="B14">
+        <f>142*5</f>
+        <v>710</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f>20*5</f>
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <f>A14-B14-C14-D14</f>
+        <v>150</v>
+      </c>
+      <c r="F14">
+        <f>E14/5</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted table cell content alignment to left-aligned for readability.
</commit_message>
<xml_diff>
--- a/planetData.xlsx
+++ b/planetData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2242a4c7a55b2ae1/Homework/ITM 361 - Web Development/Github/ITMD361_Lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{5A13FC9C-BB62-499F-8090-1424E5FBE2E4}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{8AA7C12D-2ED4-411B-99B6-9634FE8DD64B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{32DDA8C2-1474-4867-B5E3-D5AD3FDC3CA8}"/>
   </bookViews>
@@ -161,13 +161,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,7 +489,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +518,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -532,7 +535,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1">
@@ -549,7 +552,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1">
@@ -566,7 +569,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
@@ -583,7 +586,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -600,7 +603,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -617,7 +620,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1">

</xml_diff>

<commit_message>
added pulse animation for my star background to make it look like the stars are blinking
</commit_message>
<xml_diff>
--- a/planetData.xlsx
+++ b/planetData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2242a4c7a55b2ae1/Homework/ITM 361 - Web Development/Github/ITMD361_Lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{8AA7C12D-2ED4-411B-99B6-9634FE8DD64B}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{C3A35823-3DDC-4FE0-86C8-C834A5779327}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{32DDA8C2-1474-4867-B5E3-D5AD3FDC3CA8}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
finished animations for the planets
I wanted to play around with CSS animations, so I made my four planets orbit my table. The frequency of revolution and size of the planets are actually to scale (relative to Earth).
</commit_message>
<xml_diff>
--- a/planetData.xlsx
+++ b/planetData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2242a4c7a55b2ae1/Homework/ITM 361 - Web Development/Github/ITMD361_Lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{C3A35823-3DDC-4FE0-86C8-C834A5779327}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="BF06B1501B0411230003D16F83E7539FAC719FDE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{DAC731CE-4DFE-44F1-85DF-1107D19017AA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{32DDA8C2-1474-4867-B5E3-D5AD3FDC3CA8}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>1 (23.93 hours)</t>
   </si>
   <si>
-    <t>Revolution period (length of year in Earth days)</t>
-  </si>
-  <si>
     <t>5.98 x 1024</t>
   </si>
   <si>
@@ -118,13 +115,16 @@
   </si>
   <si>
     <t>Per</t>
+  </si>
+  <si>
+    <t>Revolution period (length of year in Earth years)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +134,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -161,16 +168,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,31 +497,32 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -521,50 +530,50 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>12756</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>142800</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>120660</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>49528</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
         <v>5520</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1314</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>690</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>1640</v>
       </c>
     </row>
@@ -572,16 +581,16 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>11200</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>59500</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>35600</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>23300</v>
       </c>
     </row>
@@ -589,93 +598,93 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4">
         <v>365.26</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>11.86</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>29.46</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>960</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <f>142*5</f>
         <v>710</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <f>20*5</f>
         <v>100</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <f>A14-B14-C14-D14</f>
         <v>150</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <f>E14/5</f>
         <v>30</v>
       </c>

</xml_diff>